<commit_message>
found a way to implement university search
</commit_message>
<xml_diff>
--- a/UniMatch/data/database/dataset.xlsx
+++ b/UniMatch/data/database/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\UniMatch\UniMatch\data\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB048E70-B1B9-4502-A76D-16A747B68646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A53C83-AA8B-4B75-A4B4-E01170E56F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5352" yWindow="348" windowWidth="17280" windowHeight="7608" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="1420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="1421">
   <si>
     <t>IDUser</t>
   </si>
@@ -4313,6 +4313,9 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>MainArea</t>
   </si>
 </sst>
 </file>
@@ -4754,7 +4757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408059FF-08A1-4568-82B0-C329AA08C12A}">
   <dimension ref="A1:B247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6814,15 +6817,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6841,8 +6844,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6861,8 +6867,11 @@
       <c r="F2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6881,8 +6890,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6901,8 +6913,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6921,8 +6936,11 @@
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6941,8 +6959,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6961,8 +6982,11 @@
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6981,8 +7005,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7001,8 +7028,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7021,8 +7051,11 @@
       <c r="F10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7040,6 +7073,9 @@
       </c>
       <c r="F11">
         <v>1</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>